<commit_message>
mejoras en los colores
</commit_message>
<xml_diff>
--- a/realizaciones.xlsx
+++ b/realizaciones.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\integ\kpi-architecture-ans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0C421E-D680-4267-9477-E83CA15C4FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A02DBC7-B840-4CE8-85F1-22A6FF009F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41790" yWindow="-16305" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Janvier" sheetId="3" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Janvier!$A$1:$J$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Janvier!$A$1:$L$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="146">
   <si>
     <t>Document</t>
   </si>
@@ -237,13 +238,311 @@
   </si>
   <si>
     <t>validacion/redaccion.</t>
+  </si>
+  <si>
+    <t>MaCertifPS</t>
+  </si>
+  <si>
+    <t>Resumen Project</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Ma Certif' Pro Santé/.../👥 Equipe/Règle de Vie de l’équipe</t>
+  </si>
+  <si>
+    <t>Ma Certif' Pro Santé/.../[✔️]🧰Outillage/Comment créer des diagrammes de cas d’utili</t>
+  </si>
+  <si>
+    <t>Ma Certif' Pro Santé/.../[✔️]🧰Outillage</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>Ma Certif' Pro Santé/.../Agilité/Definition Of Ready</t>
+  </si>
+  <si>
+    <t>Ma Certif' Pro Santé/.../Agilité/Definition Of Done</t>
+  </si>
+  <si>
+    <t>Ma Certif' Pro Santé/.../Agilité/Template Artefacts</t>
+  </si>
+  <si>
+    <t>Ma Certif' Pro Santé/.../📈 Méthodologie/Processus</t>
+  </si>
+  <si>
+    <t>ANS-MaCertifPS-DAF-v1.0.0-03-04-24.pdf</t>
+  </si>
+  <si>
+    <t>redaction/validation</t>
+  </si>
+  <si>
+    <t>ANS_SI-Certification-PS_Benchmark-CSP_v2.1.pdf</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>ANS_EdB_MACERTIFPS_v0.1.docx</t>
+  </si>
+  <si>
+    <t>Expression de besoin pour l’étude CSP et documentation.pptx</t>
+  </si>
+  <si>
+    <t>pptx</t>
+  </si>
+  <si>
+    <t>ANS-MaCertifPS-DAL-v1.0.0-03-04-24.pdf</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>ANS-MaCertifPS-DAT-v1.0.1-12-04-24.docx
+ANS - Ma Certification Pro - Echanges et questions.xlsx
+Draft - Subnet &amp; VLAN (1).xlsx
+ANS MaCertifPro - Estimation Dimensionnement v1 (1).xlsx</t>
+  </si>
+  <si>
+    <t>Restitution du DAL et DAT v1.0.pptx</t>
+  </si>
+  <si>
+    <t>Liste des exigences techniques comprise dans le marché.pptx</t>
+  </si>
+  <si>
+    <t>Choix Scenario Démarrage Développement.pptx</t>
+  </si>
+  <si>
+    <t>Choix du scénario pour la Transition vers la Production et Développement Continu après le POC</t>
+  </si>
+  <si>
+    <t>Atelier Cadrage pour lancer une expérimentation ​</t>
+  </si>
+  <si>
+    <t>docx</t>
+  </si>
+  <si>
+    <t>ANS_2021-05_Lot 2_MS01_SI Ma Certif Pro Sante_Cahier des Charges_V1.0-SAMER.docx</t>
+  </si>
+  <si>
+    <t>Les roles et Matrice de Compétences par rôle.</t>
+  </si>
+  <si>
+    <t>Préparation à l’homologation sécurité</t>
+  </si>
+  <si>
+    <t>Ma Certif' Pro Santé/.../En cour de 📝/🌱Écoconception Numériques pour Ma Certif P</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>Documents validés</t>
+  </si>
+  <si>
+    <t>16-31 Jan.</t>
+  </si>
+  <si>
+    <t>01-15 Feb.</t>
+  </si>
+  <si>
+    <t>16-29 Feb.</t>
+  </si>
+  <si>
+    <t>01-15 Mar.</t>
+  </si>
+  <si>
+    <t>16-31 Mar.</t>
+  </si>
+  <si>
+    <t>01-15 Avr.</t>
+  </si>
+  <si>
+    <t>16-30 Avr.</t>
+  </si>
+  <si>
+    <t>01-15 Mai.</t>
+  </si>
+  <si>
+    <t>::</t>
+  </si>
+  <si>
+    <t>01-15 Jan.</t>
+  </si>
+  <si>
+    <t>Periode Creation</t>
+  </si>
+  <si>
+    <t>Periode validation</t>
+  </si>
+  <si>
+    <t>01-15 Fév.</t>
+  </si>
+  <si>
+    <t>16-29 Fév.</t>
+  </si>
+  <si>
+    <t>Période</t>
+  </si>
+  <si>
+    <t>Documents en cours de rédaction</t>
+  </si>
+  <si>
+    <t>=NB.SI.ENS(K</t>
+  </si>
+  <si>
+    <t>; "01-15 Jan."; L</t>
+  </si>
+  <si>
+    <t>; "")</t>
+  </si>
+  <si>
+    <t>; "&lt;&gt;")</t>
+  </si>
+  <si>
+    <t>; "16-31 Jan."; L</t>
+  </si>
+  <si>
+    <t>; "01-15 Fév."; L</t>
+  </si>
+  <si>
+    <t>; "16-29 Fév."; L</t>
+  </si>
+  <si>
+    <t>; "01-15 Mar."; L</t>
+  </si>
+  <si>
+    <t>; "16-31 Mar."; L</t>
+  </si>
+  <si>
+    <t>; "01-15 Avr."; L</t>
+  </si>
+  <si>
+    <t>; "16-30 Avr."; L</t>
+  </si>
+  <si>
+    <t>; "01-15 Mai."; L</t>
+  </si>
+  <si>
+    <t>16-31 Mai.</t>
+  </si>
+  <si>
+    <t>; "16-31 Mai."; L</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel/📚 Bonnes pratiques générales/[✔️]⚖️Professionnalisme, la productivi</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel/📚 Bonnes pratiques générales/🌱Utilisation du Référentiel Général d'Écoconception de Services Numériques (RGESN) comme Bonne Pratique</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel//Générale/[✔️]🔨 Utilisation des principes SOLID</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+/
+Générale
+/
+[📝]📖 Lisibilité et maintenabilité du code</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+/
+Générale
+/
+[✔️] 📝 Documentation</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+/
+Générale
+/
+[📝]🔒 Sécurité</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+/
+Générale
+/
+[📝]🚀 Performan</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+🌟 Bonnes pratiques Code
+/
+☕ Java</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+🌟 Bonnes pratiques Code
+/
+[📝] 🅰️ Angular</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+/
+[📝] 🅰️ Angular
+/
+[📝] 🔗 Data binding, pipes</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+/
+[📝] 🅰️ Angular
+/
+[📝] 📝 Formulaires</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+/
+[📝] 🅰️ Angular
+/
+[📝] 🎨 Bonnes pratiques design</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+/
+[📝] 🅰️ Angular
+/
+[📝] 🌐 Internationalisation</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+/
+🔗 Intégration Java/Angular
+/
+[✏️]Gestion des APIs</t>
+  </si>
+  <si>
+    <t>Encyclopédie des Meilleures Pratiques en Développement Logiciel
+/
+[📝]📘 Gestion du Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +554,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -277,10 +584,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -294,8 +602,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -312,9 +637,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -352,7 +677,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -458,7 +783,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -600,7 +925,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -608,22 +933,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:F14"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" customWidth="1"/>
-    <col min="4" max="4" width="67.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.1796875" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="84.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -654,8 +988,23 @@
       <c r="J1" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -686,8 +1035,47 @@
       <c r="J2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" t="str">
+        <f>IF(AND(MONTH(E2)=1, DAY(E2)&lt;=15), "01-15 Jan.",
+IF(AND(MONTH(E2)=1, DAY(E2)&gt;=16), "16-31 Jan.",
+IF(AND(MONTH(E2)=2, DAY(E2)&lt;=15), "01-15 Fév.",
+IF(AND(MONTH(E2)=2, DAY(E2)&gt;=16), "16-29 Fév.",
+IF(AND(MONTH(E2)=3, DAY(E2)&lt;=15), "01-15 Mar.",
+IF(AND(MONTH(E2)=3, DAY(E2)&gt;=16), "16-31 Mar.",
+IF(AND(MONTH(E2)=4, DAY(E2)&lt;=15), "01-15 Avr.",
+IF(AND(MONTH(E2)=4, DAY(E2)&gt;=16), "16-30 Avr.",
+IF(AND(MONTH(E2)=5, DAY(E2)&lt;=15), "01-15 Mai.",
+IF(AND(MONTH(E2)=5, DAY(E2)&gt;=16), "16-31 Mai.",
+"01-15 Jan."))))))))))</f>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(AND(MONTH(F2)=1, DAY(F2)&lt;=15), "01-15 Jan.",
+IF(AND(MONTH(F2)=1, DAY(F2)&gt;=16), "16-31 Jan.",
+IF(AND(MONTH(F2)=2, DAY(F2)&lt;=15), "01-15 Fév.",
+IF(AND(MONTH(F2)=2, DAY(F2)&gt;=16), "16-29 Fév.",
+IF(AND(MONTH(F2)=3, DAY(F2)&lt;=15), "01-15 Mar.",
+IF(AND(MONTH(F2)=3, DAY(F2)&gt;=16), "16-31 Mar.",
+IF(AND(MONTH(F2)=4, DAY(F2)&lt;=15), "01-15 Avr.",
+IF(AND(MONTH(F2)=4, DAY(F2)&gt;=16), "16-30 Avr.",
+IF(AND(MONTH(F2)=5, DAY(F2)&lt;=15), "01-15 Mai.",
+IF(AND(MONTH(F2)=5, DAY(F2)&gt;=16), "16-31 Mai.",
+"en cours"))))))))))</f>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="O2">
+        <f>COUNTIFS(K:K,N2,L:L,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <f>COUNTIFS(K:K,N2,L:L,"&lt;&gt;")</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -703,6 +1091,9 @@
       <c r="E3" s="2">
         <v>45334</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G3" s="2">
         <v>45419</v>
       </c>
@@ -712,8 +1103,47 @@
       <c r="J3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K66" si="0">IF(AND(MONTH(E3)=1, DAY(E3)&lt;=15), "01-15 Jan.",
+IF(AND(MONTH(E3)=1, DAY(E3)&gt;=16), "16-31 Jan.",
+IF(AND(MONTH(E3)=2, DAY(E3)&lt;=15), "01-15 Fév.",
+IF(AND(MONTH(E3)=2, DAY(E3)&gt;=16), "16-29 Fév.",
+IF(AND(MONTH(E3)=3, DAY(E3)&lt;=15), "01-15 Mar.",
+IF(AND(MONTH(E3)=3, DAY(E3)&gt;=16), "16-31 Mar.",
+IF(AND(MONTH(E3)=4, DAY(E3)&lt;=15), "01-15 Avr.",
+IF(AND(MONTH(E3)=4, DAY(E3)&gt;=16), "16-30 Avr.",
+IF(AND(MONTH(E3)=5, DAY(E3)&lt;=15), "01-15 Mai.",
+IF(AND(MONTH(E3)=5, DAY(E3)&gt;=16), "16-31 Mai.",
+"01-15 Jan."))))))))))</f>
+        <v>01-15 Fév.</v>
+      </c>
+      <c r="L3" t="e">
+        <f t="shared" ref="L3:L66" si="1">IF(AND(MONTH(F3)=1, DAY(F3)&lt;=15), "01-15 Jan.",
+IF(AND(MONTH(F3)=1, DAY(F3)&gt;=16), "16-31 Jan.",
+IF(AND(MONTH(F3)=2, DAY(F3)&lt;=15), "01-15 Fév.",
+IF(AND(MONTH(F3)=2, DAY(F3)&gt;=16), "16-29 Fév.",
+IF(AND(MONTH(F3)=3, DAY(F3)&lt;=15), "01-15 Mar.",
+IF(AND(MONTH(F3)=3, DAY(F3)&gt;=16), "16-31 Mar.",
+IF(AND(MONTH(F3)=4, DAY(F3)&lt;=15), "01-15 Avr.",
+IF(AND(MONTH(F3)=4, DAY(F3)&gt;=16), "16-30 Avr.",
+IF(AND(MONTH(F3)=5, DAY(F3)&lt;=15), "01-15 Mai.",
+IF(AND(MONTH(F3)=5, DAY(F3)&gt;=16), "16-31 Mai.",
+"en cours"))))))))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O11" si="2">COUNTIFS(K:K,N3,L:L,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P11" si="3">COUNTIFS(K:K,N3,L:L,"&lt;&gt;")</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -741,8 +1171,27 @@
       <c r="J4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Fév.</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Mar.</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -770,8 +1219,27 @@
       <c r="J5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>16-29 Fév.</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="1"/>
+        <v>16-30 Avr.</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -787,6 +1255,9 @@
       <c r="E6" s="2">
         <v>45349</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G6" s="2">
         <v>45419</v>
       </c>
@@ -796,8 +1267,27 @@
       <c r="J6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>16-29 Fév.</v>
+      </c>
+      <c r="L6" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -813,6 +1303,9 @@
       <c r="E7" s="2">
         <v>45352</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G7" s="2">
         <v>45419</v>
       </c>
@@ -825,8 +1318,27 @@
       <c r="J7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Mar.</v>
+      </c>
+      <c r="L7" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -842,6 +1354,9 @@
       <c r="E8" s="2">
         <v>45355</v>
       </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G8" s="2">
         <v>45419</v>
       </c>
@@ -851,8 +1366,27 @@
       <c r="J8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Mar.</v>
+      </c>
+      <c r="L8" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -868,6 +1402,9 @@
       <c r="E9" s="2">
         <v>45362</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G9" s="2">
         <v>45419</v>
       </c>
@@ -877,8 +1414,27 @@
       <c r="J9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Mar.</v>
+      </c>
+      <c r="L9" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -894,6 +1450,9 @@
       <c r="E10" s="2">
         <v>45379</v>
       </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G10" s="2">
         <v>45419</v>
       </c>
@@ -903,8 +1462,27 @@
       <c r="J10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Mar.</v>
+      </c>
+      <c r="L10" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -929,8 +1507,27 @@
       <c r="J11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -955,8 +1552,16 @@
       <c r="J12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Fév.</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -984,37 +1589,50 @@
       <c r="J13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="1"/>
+        <v>16-29 Fév.</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="E14" s="2">
-        <v>45200</v>
+        <v>45316</v>
       </c>
       <c r="F14" s="2">
-        <v>45351</v>
-      </c>
-      <c r="H14" t="s">
-        <v>37</v>
+        <v>45425</v>
       </c>
       <c r="I14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Mai.</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1025,22 +1643,33 @@
         <v>31</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="2">
-        <v>45316</v>
+        <v>45407</v>
       </c>
       <c r="F15" s="2">
-        <v>45425</v>
+        <v>45414</v>
+      </c>
+      <c r="G15" s="2">
+        <v>45419</v>
       </c>
       <c r="I15" t="s">
         <v>38</v>
       </c>
       <c r="J15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>16-30 Avr.</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Mai.</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1051,13 +1680,13 @@
         <v>31</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E16" s="2">
         <v>45407</v>
       </c>
-      <c r="F16" s="2">
-        <v>45414</v>
+      <c r="F16" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="G16" s="2">
         <v>45419</v>
@@ -1068,8 +1697,16 @@
       <c r="J16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>16-30 Avr.</v>
+      </c>
+      <c r="L16" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1080,10 +1717,13 @@
         <v>31</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E17" s="2">
-        <v>45407</v>
+        <v>45414</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="G17" s="2">
         <v>45419</v>
@@ -1094,8 +1734,16 @@
       <c r="J17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Mai.</v>
+      </c>
+      <c r="L17" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1103,25 +1751,36 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="E18" s="2">
-        <v>45414</v>
-      </c>
-      <c r="G18" s="2">
-        <v>45419</v>
+        <v>45299</v>
+      </c>
+      <c r="F18" s="2">
+        <v>45317</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Jan.</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1132,25 +1791,33 @@
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E19" s="2">
         <v>45299</v>
       </c>
       <c r="F19" s="2">
-        <v>45317</v>
+        <v>45331</v>
       </c>
       <c r="H19" t="s">
         <v>21</v>
       </c>
       <c r="I19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Fév.</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1161,7 +1828,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" s="2">
         <v>45299</v>
@@ -1173,13 +1840,21 @@
         <v>21</v>
       </c>
       <c r="I20" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Fév.</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1190,83 +1865,107 @@
         <v>17</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E21" s="2">
-        <v>45299</v>
+        <v>45331</v>
       </c>
       <c r="F21" s="2">
-        <v>45331</v>
+        <v>45352</v>
       </c>
       <c r="H21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Fév.</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Mar.</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="2">
+        <v>110945</v>
+      </c>
+      <c r="F22" s="2">
+        <v>45239</v>
+      </c>
+      <c r="H22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="1"/>
+        <v>en cours</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E23" s="2">
         <v>45331</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F23" s="2">
         <v>45352</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H23" t="s">
         <v>22</v>
       </c>
-      <c r="I22" t="s">
-        <v>24</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="I23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="2">
-        <v>110945</v>
-      </c>
-      <c r="F23" s="2">
-        <v>45239</v>
-      </c>
-      <c r="H23" t="s">
-        <v>37</v>
-      </c>
-      <c r="I23" t="s">
-        <v>38</v>
-      </c>
-      <c r="J23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Fév.</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Mar.</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1289,13 +1988,21 @@
         <v>22</v>
       </c>
       <c r="I24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J24" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Fév.</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Mar.</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1303,48 +2010,56 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E25" s="2">
-        <v>45331</v>
+        <v>45309</v>
       </c>
       <c r="F25" s="2">
-        <v>45352</v>
+        <v>45365</v>
       </c>
       <c r="H25" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="I25" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="J25" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Mar.</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E26" s="2">
-        <v>45309</v>
+        <v>45196</v>
       </c>
       <c r="F26" s="2">
-        <v>45365</v>
+        <v>45369</v>
       </c>
       <c r="H26" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I26" t="s">
         <v>35</v>
@@ -1352,37 +2067,53 @@
       <c r="J26" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Mar.</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E27" s="2">
-        <v>45196</v>
+        <v>45320</v>
       </c>
       <c r="F27" s="2">
         <v>45369</v>
       </c>
       <c r="H27" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Mar.</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1393,16 +2124,16 @@
         <v>31</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E28" s="2">
-        <v>45320</v>
+        <v>45322</v>
       </c>
       <c r="F28" s="2">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="H28" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I28" t="s">
         <v>38</v>
@@ -1410,8 +2141,16 @@
       <c r="J28" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Mar.</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1419,28 +2158,36 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="E29" s="2">
-        <v>45322</v>
+        <v>45337</v>
       </c>
       <c r="F29" s="2">
-        <v>45370</v>
+        <v>45407</v>
       </c>
       <c r="H29" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="I29" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="J29" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K29" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Fév.</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="1"/>
+        <v>16-30 Avr.</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1448,59 +2195,75 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E30" s="2">
-        <v>45337</v>
-      </c>
-      <c r="F30" s="2">
-        <v>45407</v>
+        <v>44999</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="H30" t="s">
         <v>21</v>
       </c>
       <c r="I30" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J30" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Mar.</v>
+      </c>
+      <c r="L30" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E31" s="2">
-        <v>44999</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" t="s">
-        <v>21</v>
+        <v>45373</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="2">
+        <v>45419</v>
       </c>
       <c r="I31" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Mar.</v>
+      </c>
+      <c r="L31" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -1509,32 +2272,2466 @@
         <v>31</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="E32" s="2">
-        <v>45373</v>
-      </c>
-      <c r="G32" s="2">
-        <v>45419</v>
+        <v>45313</v>
+      </c>
+      <c r="F32" s="2">
+        <v>45313</v>
+      </c>
+      <c r="H32" t="s">
+        <v>21</v>
       </c>
       <c r="I32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="K32" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Jan.</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="2">
+        <v>45313</v>
+      </c>
+      <c r="F33" s="2">
+        <v>45314</v>
+      </c>
+      <c r="H33" t="s">
+        <v>72</v>
+      </c>
+      <c r="I33" t="s">
+        <v>38</v>
+      </c>
+      <c r="J33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Jan.</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="2">
+        <v>45278</v>
+      </c>
+      <c r="F34" s="2">
+        <v>45314</v>
+      </c>
+      <c r="H34" t="s">
+        <v>86</v>
+      </c>
+      <c r="I34" t="s">
+        <v>38</v>
+      </c>
+      <c r="J34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Jan.</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="2">
+        <v>45331</v>
+      </c>
+      <c r="F35" s="2">
+        <v>45331</v>
+      </c>
+      <c r="H35" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" t="s">
+        <v>38</v>
+      </c>
+      <c r="J35" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Fév.</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Fév.</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="2">
+        <v>45313</v>
+      </c>
+      <c r="F36" s="2">
+        <v>45336</v>
+      </c>
+      <c r="H36" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" t="s">
+        <v>35</v>
+      </c>
+      <c r="J36" t="s">
+        <v>33</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Fév.</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="2">
+        <v>45282</v>
+      </c>
+      <c r="F37" s="2">
+        <v>45338</v>
+      </c>
+      <c r="H37" t="s">
+        <v>86</v>
+      </c>
+      <c r="I37" t="s">
+        <v>38</v>
+      </c>
+      <c r="J37" t="s">
+        <v>78</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="1"/>
+        <v>16-29 Fév.</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="2">
+        <v>45338</v>
+      </c>
+      <c r="F38" s="2">
+        <v>45358</v>
+      </c>
+      <c r="H38" t="s">
+        <v>72</v>
+      </c>
+      <c r="I38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J38" t="s">
+        <v>78</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="0"/>
+        <v>16-29 Fév.</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Mar.</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="2">
+        <v>45377</v>
+      </c>
+      <c r="F39" s="2">
+        <v>45380</v>
+      </c>
+      <c r="H39" t="s">
+        <v>86</v>
+      </c>
+      <c r="I39" t="s">
+        <v>38</v>
+      </c>
+      <c r="J39" t="s">
+        <v>33</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Mar.</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Mar.</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="2">
+        <v>45275</v>
+      </c>
+      <c r="F40" s="2">
+        <v>45310</v>
+      </c>
+      <c r="H40" t="s">
+        <v>81</v>
+      </c>
+      <c r="I40" t="s">
+        <v>38</v>
+      </c>
+      <c r="J40" t="s">
+        <v>34</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Jan.</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="2">
+        <v>45313</v>
+      </c>
+      <c r="F41" s="2">
+        <v>45385</v>
+      </c>
+      <c r="H41" t="s">
+        <v>45</v>
+      </c>
+      <c r="I41" t="s">
+        <v>35</v>
+      </c>
+      <c r="J41" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Avr.</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="2">
+        <v>45328</v>
+      </c>
+      <c r="F42" s="2">
+        <v>45331</v>
+      </c>
+      <c r="H42" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" t="s">
+        <v>38</v>
+      </c>
+      <c r="J42" t="s">
+        <v>34</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Fév.</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Fév.</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="2">
+        <v>45313</v>
+      </c>
+      <c r="F43" s="2">
+        <v>45385</v>
+      </c>
+      <c r="H43" t="s">
+        <v>68</v>
+      </c>
+      <c r="I43" t="s">
+        <v>35</v>
+      </c>
+      <c r="J43" t="s">
+        <v>33</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Avr.</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" s="2">
+        <v>45338</v>
+      </c>
+      <c r="F44" s="2">
+        <v>45385</v>
+      </c>
+      <c r="H44" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" t="s">
+        <v>34</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="0"/>
+        <v>16-29 Fév.</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Avr.</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="2">
+        <v>45313</v>
+      </c>
+      <c r="F45" s="2">
+        <v>45386</v>
+      </c>
+      <c r="H45" t="s">
+        <v>68</v>
+      </c>
+      <c r="I45" t="s">
+        <v>35</v>
+      </c>
+      <c r="J45" t="s">
+        <v>33</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Avr.</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" s="2">
+        <v>45386</v>
+      </c>
+      <c r="F46" s="2">
+        <v>45390</v>
+      </c>
+      <c r="H46" t="s">
+        <v>37</v>
+      </c>
+      <c r="I46" t="s">
+        <v>38</v>
+      </c>
+      <c r="J46" t="s">
+        <v>33</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Avr.</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Avr.</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="2">
+        <v>45391</v>
+      </c>
+      <c r="F47" s="2">
+        <v>45392</v>
+      </c>
+      <c r="H47" t="s">
+        <v>86</v>
+      </c>
+      <c r="I47" t="s">
+        <v>38</v>
+      </c>
+      <c r="J47" t="s">
+        <v>33</v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Avr.</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Avr.</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="2">
+        <v>45392</v>
+      </c>
+      <c r="F48" s="2">
+        <v>45394</v>
+      </c>
+      <c r="H48" t="s">
+        <v>86</v>
+      </c>
+      <c r="I48" t="s">
+        <v>38</v>
+      </c>
+      <c r="J48" t="s">
+        <v>33</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Avr.</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Avr.</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="2">
+        <v>45393</v>
+      </c>
+      <c r="F49" s="2">
+        <v>45394</v>
+      </c>
+      <c r="H49" t="s">
+        <v>86</v>
+      </c>
+      <c r="I49" t="s">
+        <v>38</v>
+      </c>
+      <c r="J49" t="s">
+        <v>33</v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Avr.</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Avr.</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E50" s="2">
+        <v>45412</v>
+      </c>
+      <c r="F50" s="2">
+        <v>45412</v>
+      </c>
+      <c r="H50" t="s">
+        <v>86</v>
+      </c>
+      <c r="I50" t="s">
+        <v>38</v>
+      </c>
+      <c r="J50" t="s">
+        <v>33</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="0"/>
+        <v>16-30 Avr.</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="1"/>
+        <v>16-30 Avr.</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" s="2">
+        <v>45386</v>
+      </c>
+      <c r="F51" s="2">
+        <v>45394</v>
+      </c>
+      <c r="H51" t="s">
+        <v>21</v>
+      </c>
+      <c r="I51" t="s">
+        <v>38</v>
+      </c>
+      <c r="J51" t="s">
+        <v>34</v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Avr.</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Avr.</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="2">
+        <v>45418</v>
+      </c>
+      <c r="F52" s="2">
+        <v>45418</v>
+      </c>
+      <c r="H52" t="s">
+        <v>68</v>
+      </c>
+      <c r="I52" t="s">
+        <v>35</v>
+      </c>
+      <c r="J52" t="s">
+        <v>33</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Mai.</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Mai.</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E53" s="2">
+        <v>45425</v>
+      </c>
+      <c r="F53" s="2">
+        <v>45425</v>
+      </c>
+      <c r="G53" t="s">
+        <v>108</v>
+      </c>
+      <c r="H53" t="s">
+        <v>86</v>
+      </c>
+      <c r="I53" t="s">
+        <v>38</v>
+      </c>
+      <c r="J53" t="s">
+        <v>33</v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Mai.</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Mai.</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" t="s">
+        <v>98</v>
+      </c>
+      <c r="I54" t="s">
+        <v>38</v>
+      </c>
+      <c r="J54" t="s">
+        <v>33</v>
+      </c>
+      <c r="K54" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L54" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>4</v>
       </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" s="2">
+        <v>45200</v>
+      </c>
+      <c r="F55" s="2">
+        <v>45351</v>
+      </c>
+      <c r="H55" t="s">
+        <v>37</v>
+      </c>
+      <c r="I55" t="s">
+        <v>35</v>
+      </c>
+      <c r="J55" t="s">
+        <v>33</v>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="1"/>
+        <v>16-29 Fév.</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E56" s="2">
+        <v>45310</v>
+      </c>
+      <c r="F56" s="2">
+        <v>45350</v>
+      </c>
+      <c r="H56" t="s">
+        <v>132</v>
+      </c>
+      <c r="J56" t="s">
+        <v>33</v>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="1"/>
+        <v>16-29 Fév.</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E57" s="2">
+        <v>45355</v>
+      </c>
+      <c r="F57" s="2">
+        <v>45408</v>
+      </c>
+      <c r="H57" t="s">
+        <v>50</v>
+      </c>
+      <c r="J57" t="s">
+        <v>33</v>
+      </c>
+      <c r="K57" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Mar.</v>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="1"/>
+        <v>16-30 Avr.</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E58" s="2">
+        <v>45310</v>
+      </c>
+      <c r="F58" s="2">
+        <v>45350</v>
+      </c>
+      <c r="H58" t="s">
+        <v>45</v>
+      </c>
+      <c r="J58" t="s">
+        <v>34</v>
+      </c>
+      <c r="K58" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L58" t="str">
+        <f t="shared" si="1"/>
+        <v>16-29 Fév.</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E59" s="2">
+        <v>45350</v>
+      </c>
+      <c r="J59" t="s">
+        <v>78</v>
+      </c>
+      <c r="K59" t="str">
+        <f t="shared" si="0"/>
+        <v>16-29 Fév.</v>
+      </c>
+      <c r="L59" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="2">
+        <v>45311</v>
+      </c>
+      <c r="F60" s="2">
+        <v>45351</v>
+      </c>
+      <c r="K60" t="str">
+        <f>IF(AND(MONTH(F60)=1, DAY(F60)&lt;=15), "01-15 Jan.",
+IF(AND(MONTH(F60)=1, DAY(F60)&gt;=16), "16-31 Jan.",
+IF(AND(MONTH(F60)=2, DAY(F60)&lt;=15), "01-15 Fév.",
+IF(AND(MONTH(F60)=2, DAY(F60)&gt;=16), "16-29 Fév.",
+IF(AND(MONTH(F60)=3, DAY(F60)&lt;=15), "01-15 Mar.",
+IF(AND(MONTH(F60)=3, DAY(F60)&gt;=16), "16-31 Mar.",
+IF(AND(MONTH(F60)=4, DAY(F60)&lt;=15), "01-15 Avr.",
+IF(AND(MONTH(F60)=4, DAY(F60)&gt;=16), "16-30 Avr.",
+IF(AND(MONTH(F60)=5, DAY(F60)&lt;=15), "01-15 Mai.",
+IF(AND(MONTH(F60)=5, DAY(F60)&gt;=16), "16-31 Mai.",
+"01-15 Jan."))))))))))</f>
+        <v>16-29 Fév.</v>
+      </c>
+      <c r="L60" t="str">
+        <f t="shared" si="1"/>
+        <v>16-29 Fév.</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E61" s="2">
+        <v>45311</v>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>31</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62" s="2">
+        <v>45311</v>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L62" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E63" s="2">
+        <v>45225</v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L63" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E64" s="2">
+        <v>45225</v>
+      </c>
+      <c r="F64" s="2">
+        <v>45317</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="0"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L64" t="str">
+        <f t="shared" si="1"/>
+        <v>16-31 Jan.</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
+        <v>31</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E65" s="2">
+        <v>45315</v>
+      </c>
+      <c r="K65" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L65" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
+        <v>31</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E66" s="2">
+        <v>45315</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="0"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L66" t="str">
+        <f t="shared" si="1"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E67" s="2">
+        <v>45317</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K78" si="4">IF(AND(MONTH(E67)=1, DAY(E67)&lt;=15), "01-15 Jan.",
+IF(AND(MONTH(E67)=1, DAY(E67)&gt;=16), "16-31 Jan.",
+IF(AND(MONTH(E67)=2, DAY(E67)&lt;=15), "01-15 Fév.",
+IF(AND(MONTH(E67)=2, DAY(E67)&gt;=16), "16-29 Fév.",
+IF(AND(MONTH(E67)=3, DAY(E67)&lt;=15), "01-15 Mar.",
+IF(AND(MONTH(E67)=3, DAY(E67)&gt;=16), "16-31 Mar.",
+IF(AND(MONTH(E67)=4, DAY(E67)&lt;=15), "01-15 Avr.",
+IF(AND(MONTH(E67)=4, DAY(E67)&gt;=16), "16-30 Avr.",
+IF(AND(MONTH(E67)=5, DAY(E67)&lt;=15), "01-15 Mai.",
+IF(AND(MONTH(E67)=5, DAY(E67)&gt;=16), "16-31 Mai.",
+"01-15 Jan."))))))))))</f>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L67" t="str">
+        <f t="shared" ref="L67:L78" si="5">IF(AND(MONTH(F67)=1, DAY(F67)&lt;=15), "01-15 Jan.",
+IF(AND(MONTH(F67)=1, DAY(F67)&gt;=16), "16-31 Jan.",
+IF(AND(MONTH(F67)=2, DAY(F67)&lt;=15), "01-15 Fév.",
+IF(AND(MONTH(F67)=2, DAY(F67)&gt;=16), "16-29 Fév.",
+IF(AND(MONTH(F67)=3, DAY(F67)&lt;=15), "01-15 Mar.",
+IF(AND(MONTH(F67)=3, DAY(F67)&gt;=16), "16-31 Mar.",
+IF(AND(MONTH(F67)=4, DAY(F67)&lt;=15), "01-15 Avr.",
+IF(AND(MONTH(F67)=4, DAY(F67)&gt;=16), "16-30 Avr.",
+IF(AND(MONTH(F67)=5, DAY(F67)&lt;=15), "01-15 Mai.",
+IF(AND(MONTH(F67)=5, DAY(F67)&gt;=16), "16-31 Mai.",
+"en cours"))))))))))</f>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E68" s="2">
+        <v>45317</v>
+      </c>
+      <c r="K68" t="str">
+        <f t="shared" si="4"/>
+        <v>16-31 Jan.</v>
+      </c>
+      <c r="L68" t="str">
+        <f t="shared" si="5"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" s="2">
+        <v>45204</v>
+      </c>
+      <c r="F69" s="2">
+        <v>45350</v>
+      </c>
+      <c r="K69" t="str">
+        <f t="shared" si="4"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L69" t="str">
+        <f t="shared" si="5"/>
+        <v>16-29 Fév.</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" t="s">
+        <v>31</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" s="2">
+        <v>45350</v>
+      </c>
+      <c r="F70" s="2">
+        <v>45393</v>
+      </c>
+      <c r="K70" t="str">
+        <f t="shared" si="4"/>
+        <v>16-29 Fév.</v>
+      </c>
+      <c r="L70" t="str">
+        <f t="shared" si="5"/>
+        <v>01-15 Avr.</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" t="s">
+        <v>31</v>
+      </c>
+      <c r="K71" t="str">
+        <f t="shared" si="4"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L71" t="str">
+        <f t="shared" si="5"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
+        <v>31</v>
+      </c>
+      <c r="K72" t="str">
+        <f t="shared" si="4"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L72" t="str">
+        <f t="shared" si="5"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>31</v>
+      </c>
+      <c r="K73" t="str">
+        <f t="shared" si="4"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L73" t="str">
+        <f t="shared" si="5"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>31</v>
+      </c>
+      <c r="K74" t="str">
+        <f t="shared" si="4"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L74" t="str">
+        <f t="shared" si="5"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>31</v>
+      </c>
+      <c r="K75" t="str">
+        <f t="shared" si="4"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L75" t="str">
+        <f t="shared" si="5"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>31</v>
+      </c>
+      <c r="K76" t="str">
+        <f t="shared" si="4"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L76" t="str">
+        <f t="shared" si="5"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K77" t="str">
+        <f t="shared" si="4"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L77" t="str">
+        <f t="shared" si="5"/>
+        <v>01-15 Jan.</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K78" t="str">
+        <f t="shared" si="4"/>
+        <v>01-15 Jan.</v>
+      </c>
+      <c r="L78" t="str">
+        <f t="shared" si="5"/>
+        <v>01-15 Jan.</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J33" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J32">
-      <sortCondition ref="F1:F33"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:L70" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <hyperlinks>
+    <hyperlink ref="D38" r:id="rId1" tooltip="https://esantegouv.sharepoint.com/:b:/r/sites/GED-Calypso/espace-projets/Espace%20SI%20CertifPS/03-Produit%20SI%20Certif%20PS/01-Conception/Technique/Etude/02%20DAF-DAL-DAT/ANS-MaCertifPS-DAF-v1.0.0-03-04-24.pdf?csf=1&amp;web=1&amp;e=dKcpNt" display="https://esantegouv.sharepoint.com/:b:/r/sites/GED-Calypso/espace-projets/Espace SI CertifPS/03-Produit SI Certif PS/01-Conception/Technique/Etude/02 DAF-DAL-DAT/ANS-MaCertifPS-DAF-v1.0.0-03-04-24.pdf?csf=1&amp;web=1&amp;e=dKcpNt" xr:uid="{31EAB6E5-5DD6-45C6-9909-0D8E4EA0903C}"/>
+    <hyperlink ref="D40" r:id="rId2" tooltip="https://esantegouv.sharepoint.com/:b:/r/sites/GED-Calypso/espace-projets/Espace%20SI%20CertifPS/03-Produit%20SI%20Certif%20PS/01-Conception/Technique/Etude/01%20Choix%20CSP/ANS_SI-Certification-PS_Benchmark-CSP_v2.1.pdf?csf=1&amp;web=1&amp;e=fZaI8p" display="https://esantegouv.sharepoint.com/:b:/r/sites/GED-Calypso/espace-projets/Espace SI CertifPS/03-Produit SI Certif PS/01-Conception/Technique/Etude/01 Choix CSP/ANS_SI-Certification-PS_Benchmark-CSP_v2.1.pdf?csf=1&amp;web=1&amp;e=fZaI8p" xr:uid="{C032419D-D6C3-4426-B60F-CF6E0785E933}"/>
+    <hyperlink ref="D51" r:id="rId3" tooltip="https://esantegouv.sharepoint.com/:w:/r/sites/GED-Calypso/espace-projets/Espace%20SI%20CertifPS/03-Produit%20SI%20Certif%20PS/01-Conception/Technique/Etude/02%20DAF-DAL-DAT/ANS-MaCertifPS-DAT-v1.0.1-12-04-24.docx?d=wd80c4eddab864af2a0548bdb2da48410&amp;csf=1&amp;" display="https://esantegouv.sharepoint.com/:w:/r/sites/GED-Calypso/espace-projets/Espace SI CertifPS/03-Produit SI Certif PS/01-Conception/Technique/Etude/02 DAF-DAL-DAT/ANS-MaCertifPS-DAT-v1.0.1-12-04-24.docx?d=wd80c4eddab864af2a0548bdb2da48410&amp;csf=1&amp;web=1&amp;e=oa1UwS" xr:uid="{0982EBF6-4DBD-4136-9374-36D6AE44A39E}"/>
+    <hyperlink ref="D48" r:id="rId4" tooltip="https://esantegouv.sharepoint.com/:p:/r/sites/GED-Calypso/espace-projets/Espace%20SI%20CertifPS/03-Produit%20SI%20Certif%20PS/01-Conception/Technique/Restitution%20du%20DAL%20et%20DAT%20v1.0.pptx?d=wd21a8ebfff814ba2972355a23a1d04fd&amp;csf=1&amp;web=1&amp;e=5rts51" display="https://esantegouv.sharepoint.com/:p:/r/sites/GED-Calypso/espace-projets/Espace SI CertifPS/03-Produit SI Certif PS/01-Conception/Technique/Restitution du DAL et DAT v1.0.pptx?d=wd21a8ebfff814ba2972355a23a1d04fd&amp;csf=1&amp;web=1&amp;e=5rts51" xr:uid="{2A1437A4-884A-4130-98EE-3CCAA2B09D82}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98063256-F2C2-4532-A35D-6E714A180DA9}">
+  <dimension ref="A1:L50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="51.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45334</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45419</v>
+      </c>
+      <c r="I2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45335</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45377</v>
+      </c>
+      <c r="G3" s="2">
+        <v>45419</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45349</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45407</v>
+      </c>
+      <c r="G4" s="2">
+        <v>45419</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="2">
+        <v>45349</v>
+      </c>
+      <c r="G5" s="2">
+        <v>45419</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="2">
+        <v>45352</v>
+      </c>
+      <c r="G6" s="2">
+        <v>45419</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="2">
+        <v>45355</v>
+      </c>
+      <c r="G7" s="2">
+        <v>45419</v>
+      </c>
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="2">
+        <v>45362</v>
+      </c>
+      <c r="G8" s="2">
+        <v>45419</v>
+      </c>
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="2">
+        <v>45379</v>
+      </c>
+      <c r="G9" s="2">
+        <v>45419</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" t="s">
+        <v>104</v>
+      </c>
+      <c r="L9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="2">
+        <v>45407</v>
+      </c>
+      <c r="F10" s="2">
+        <v>45414</v>
+      </c>
+      <c r="G10" s="2">
+        <v>45419</v>
+      </c>
+      <c r="I10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" t="s">
+        <v>106</v>
+      </c>
+      <c r="L10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="2">
+        <v>45407</v>
+      </c>
+      <c r="G11" s="2">
+        <v>45419</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="2">
+        <v>45414</v>
+      </c>
+      <c r="G12" s="2">
+        <v>45419</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" t="s">
+        <v>107</v>
+      </c>
+      <c r="L12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2">
+        <v>45299</v>
+      </c>
+      <c r="F13" s="2">
+        <v>45317</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" t="s">
+        <v>109</v>
+      </c>
+      <c r="L13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2">
+        <v>45299</v>
+      </c>
+      <c r="F14" s="2">
+        <v>45331</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" t="s">
+        <v>109</v>
+      </c>
+      <c r="L14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="2">
+        <v>45299</v>
+      </c>
+      <c r="F15" s="2">
+        <v>45331</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" t="s">
+        <v>109</v>
+      </c>
+      <c r="L15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="2">
+        <v>45331</v>
+      </c>
+      <c r="F16" s="2">
+        <v>45352</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" t="s">
+        <v>112</v>
+      </c>
+      <c r="L16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="2">
+        <v>45331</v>
+      </c>
+      <c r="F17" s="2">
+        <v>45352</v>
+      </c>
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" t="s">
+        <v>112</v>
+      </c>
+      <c r="L17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="2">
+        <v>45331</v>
+      </c>
+      <c r="F18" s="2">
+        <v>45352</v>
+      </c>
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" t="s">
+        <v>112</v>
+      </c>
+      <c r="L18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="2">
+        <v>45309</v>
+      </c>
+      <c r="F19" s="2">
+        <v>45365</v>
+      </c>
+      <c r="H19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" t="s">
+        <v>100</v>
+      </c>
+      <c r="L19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
+      <c r="B25" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="12"/>
+      <c r="B26" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+      <c r="B28" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="12"/>
+      <c r="B35" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="12"/>
+      <c r="B37" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="12"/>
+      <c r="B38" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="12"/>
+      <c r="B40" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="12"/>
+      <c r="B41" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="12"/>
+      <c r="B43" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="12"/>
+      <c r="B44" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="12"/>
+      <c r="B46" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="12"/>
+      <c r="B47" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="12"/>
+      <c r="B49" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="12"/>
+      <c r="B50" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A38"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>